<commit_message>
Added errorbars showing std
-Added errorbars
-Added results in probability distribution and Fs
</commit_message>
<xml_diff>
--- a/2DIsing_Fs/input_Fs.xlsx
+++ b/2DIsing_Fs/input_Fs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My files\Project course\presentation\after mid sem_week 1\beta 1\final\2DIsing_Fs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prateek Verma\Documents\GitHub\2d_ising_simulation\2DIsing_Fs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" iterate="1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -407,7 +408,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -441,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -479,7 +480,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>2.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -487,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>